<commit_message>
readme and codebook update
</commit_message>
<xml_diff>
--- a/data/mema_codebook.xlsx
+++ b/data/mema_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Misinformation_meta\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RabbitSnore\Documents\Projects\Misinformation_meta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF8CC5F3-C142-4740-84AD-7B8F280D2B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2975CD7-5D7D-4684-A9C8-73104237CA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{38FE1802-D0E4-4D04-A5E5-B4F66745BCD3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{38FE1802-D0E4-4D04-A5E5-B4F66745BCD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="171">
   <si>
     <t>id_record</t>
   </si>
@@ -437,9 +437,6 @@
     <t>Delay between exposure to event and misinformation, in hours (if less than one hour, use 0; if in days, multiply days by 24)</t>
   </si>
   <si>
-    <t>perceptive nature used for misinformation exposure</t>
-  </si>
-  <si>
     <t>Method of exposure to misinformation</t>
   </si>
   <si>
@@ -449,9 +446,6 @@
     <t>Valence of the misinformation</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of recall tests conducted after the event but prior to the test effect of interest. </t>
-  </si>
-  <si>
     <t>Delay between exposure to misinformation and recall, in hours (if less than one hour, use 0; if in days, multiply days by 24)</t>
   </si>
   <si>
@@ -470,9 +464,6 @@
     <t>Central or peripheral details</t>
   </si>
   <si>
-    <t>Type of control item. Novel = only shows up on the test(control, foil, novel), Consistent - info in the event and the post event stage</t>
-  </si>
-  <si>
     <t>Number of misled items on the test</t>
   </si>
   <si>
@@ -480,6 +471,84 @@
   </si>
   <si>
     <t>Additional information about moderator coding</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>community = members of the general community; students = university students; older_adults = participants recruited specifically for being elderly; prolific = recruited from prolific.com; mturk = receruited from Mechanical Turk</t>
+  </si>
+  <si>
+    <t>lab = in a laboratory; field = outside of an academic setting; online = internet mediated</t>
+  </si>
+  <si>
+    <t>money = monetary compensation; required = required as a part of a course; none = no incentive; course_credit = academic credit; course_credit_or_money = either credit or monetary compensation; raffle = a lottery; goods = other items as incentives</t>
+  </si>
+  <si>
+    <t>0 = not registered; 1 = preregistered</t>
+  </si>
+  <si>
+    <t>0 = no claim of open data; 1 = claim of open data</t>
+  </si>
+  <si>
+    <t>0 = data not open; 1 = open data</t>
+  </si>
+  <si>
+    <t>0 = no open materials; 1 = open materials</t>
+  </si>
+  <si>
+    <t>Perceptual medium used for misinformation exposure</t>
+  </si>
+  <si>
+    <t>between = between subjects; within = within subjects</t>
+  </si>
+  <si>
+    <t>0 = not reversed; 1 = reversed</t>
+  </si>
+  <si>
+    <t>Number of control items on the test</t>
+  </si>
+  <si>
+    <t>intellectual_disability = participants are intellectually disabled; alcoholics = participants have alcoholism</t>
+  </si>
+  <si>
+    <t>no_manipulation = no manipulation of valence; negative = negative mood; neutral = neutral mood; positive = positive mood</t>
+  </si>
+  <si>
+    <t>0 = no warning; 1 = warning</t>
+  </si>
+  <si>
+    <t>0 = no correction; 1 = correction</t>
+  </si>
+  <si>
+    <t>0 = no alcohol; 1 = alcohol</t>
+  </si>
+  <si>
+    <t>visual = visual medium; audiovisual = sound and video; live = live event; text = text stimuli; audio = sound</t>
+  </si>
+  <si>
+    <t>no_manipulation = no manipulation; traumatic = event was traumatic; negative = negative valence; neutral = neutral valence; positive = positive valence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no_manipulation = no manipulation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of tests conducted after the event but prior to the test effect of interest. </t>
+  </si>
+  <si>
+    <t>recognition = recognition test; source_monitoring = source monitoring test; cued_recall = cued recall test; modified_test = modified test; interpolated_recall = interpolated recall test; free_recall = free recall; MMFR = modified modified free recall; total_recall = total recall procedure; color_recognition = color identifying task; line_up = line up identification</t>
+  </si>
+  <si>
+    <t>peripheral = peripheral details; central = central details</t>
   </si>
 </sst>
 </file>
@@ -521,9 +590,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -858,606 +928,901 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDF0301-BBC4-4423-AE5D-86F2CEAC869C}">
-  <dimension ref="A1:B74"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="J72" sqref="J72"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.73046875" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>73</v>
       </c>
       <c r="B1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>148</v>
+      </c>
+      <c r="D26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>147</v>
+      </c>
+      <c r="D30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>148</v>
+      </c>
+      <c r="D38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>147</v>
+      </c>
+      <c r="D56" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>148</v>
+      </c>
+      <c r="D58" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="C60" t="s">
+        <v>147</v>
+      </c>
+      <c r="D60" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="C61" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="C62" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="C63" t="s">
+        <v>147</v>
+      </c>
+      <c r="D63" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>62</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C64" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="C65" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="C66" t="s">
+        <v>148</v>
+      </c>
+      <c r="D66" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="C67" t="s">
+        <v>148</v>
+      </c>
+      <c r="D67" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>66</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="C68" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="C69" t="s">
+        <v>147</v>
+      </c>
+      <c r="D69" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="C70" t="s">
+        <v>147</v>
+      </c>
+      <c r="D70" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="C71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="C72" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="C73" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C74" t="s">
         <v>147</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update after new coding for revision
</commit_message>
<xml_diff>
--- a/data/mema_codebook.xlsx
+++ b/data/mema_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RabbitSnore\Documents\Projects\Misinformation_meta\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Misinformation_meta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2028233F-1CB3-4437-9F3B-5E2A7B2F1F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB331700-FFAB-4D7E-A4C1-5464757E0DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{38FE1802-D0E4-4D04-A5E5-B4F66745BCD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{38FE1802-D0E4-4D04-A5E5-B4F66745BCD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="178">
   <si>
     <t>id_record</t>
   </si>
@@ -305,15 +305,6 @@
     <t>DOI</t>
   </si>
   <si>
-    <t>language of record</t>
-  </si>
-  <si>
-    <t>language of materials</t>
-  </si>
-  <si>
-    <t>Country in which study was conducted</t>
-  </si>
-  <si>
     <t>Modality of study procedures</t>
   </si>
   <si>
@@ -344,24 +335,6 @@
     <t>Within-subjects or between-subjects comparison indicator</t>
   </si>
   <si>
-    <t>Proportion of participants with accurate report in the control condition</t>
-  </si>
-  <si>
-    <t>Proportion of participants with accurate report in the misinformation condition</t>
-  </si>
-  <si>
-    <t>Mean correct in the control condition</t>
-  </si>
-  <si>
-    <t>Mean correct in the misinformation condition</t>
-  </si>
-  <si>
-    <t>Standard deviation in the control condition</t>
-  </si>
-  <si>
-    <t>Standard deviation in the misinformation condition</t>
-  </si>
-  <si>
     <t>Type of accuracy measure for means</t>
   </si>
   <si>
@@ -374,12 +347,6 @@
     <t>Total sample size</t>
   </si>
   <si>
-    <t>Inferential test statistic</t>
-  </si>
-  <si>
-    <t>Type of statistic (e.g., t, F)</t>
-  </si>
-  <si>
     <t>Type of control items</t>
   </si>
   <si>
@@ -428,9 +395,6 @@
     <t>Valence of the event</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of recall tests conducted before exposure to PEI prior to the test effect of interest. </t>
-  </si>
-  <si>
     <t>Presence of warning about misinformation after the initial event</t>
   </si>
   <si>
@@ -461,18 +425,6 @@
     <t>Medium of test</t>
   </si>
   <si>
-    <t>Central or peripheral details</t>
-  </si>
-  <si>
-    <t>Number of misled items on the test</t>
-  </si>
-  <si>
-    <t>Total number of items on the test</t>
-  </si>
-  <si>
-    <t>Additional information about moderator coding</t>
-  </si>
-  <si>
     <t>values</t>
   </si>
   <si>
@@ -515,9 +467,6 @@
     <t>0 = not reversed; 1 = reversed</t>
   </si>
   <si>
-    <t>Number of control items on the test</t>
-  </si>
-  <si>
     <t>intellectual_disability = participants are intellectually disabled; alcoholics = participants have alcoholism</t>
   </si>
   <si>
@@ -560,10 +509,67 @@
     <t>Additional information about misinformation type</t>
   </si>
   <si>
-    <t>Type of misinformation participants were exposed</t>
-  </si>
-  <si>
     <t>additive = misinformation that adds details to the event; contradictory = misinformation that changes details in the event; mixed = a mixture of additive and contradictory; unclear = not enough information for a clear identification of the type of misinformation</t>
+  </si>
+  <si>
+    <t>Type of misinformation participants were exposed to. Note that this coding is inferred from the misinformation items provided in the reports, and this reporting often only includes a small set of examples (or no examples). As such, this coding may contain substantial error.</t>
+  </si>
+  <si>
+    <t>Additional information about moderator coding.</t>
+  </si>
+  <si>
+    <t>language of record, ISO 639 code</t>
+  </si>
+  <si>
+    <t>language of materials, ISO 639 code</t>
+  </si>
+  <si>
+    <t>Country in which study was conducted, ISO 3166 code</t>
+  </si>
+  <si>
+    <t>Proportion of participants with accurate report in the misinformation condition.  Coded when there is a single critical item and outcome is reported as a proportion.</t>
+  </si>
+  <si>
+    <t>Proportion of participants with accurate report in the control condition. Coded when there is a single critical item and outcome is reported as a proportion.</t>
+  </si>
+  <si>
+    <t>Mean correct in the control condition. Coded when outcome is reported as a mean (e.g., a mean accuracy or mean items correct).</t>
+  </si>
+  <si>
+    <t>Mean correct in the misinformation condition. Coded when outcome is reported as a mean (e.g., a mean accuracy or mean items correct).</t>
+  </si>
+  <si>
+    <t>Standard deviation in the control condition. Coded when outcome is reported as a mean (e.g., a mean accuracy or mean items correct).</t>
+  </si>
+  <si>
+    <t>Standard deviation in the misinformation condition. Coded when outcome is reported as a mean (e.g., a mean accuracy or mean items correct).</t>
+  </si>
+  <si>
+    <t>count = count of items correct/incorrect; proportion = propotion correct or proportion of participants who were accurate/inaccurate</t>
+  </si>
+  <si>
+    <t>Inferential test statistic for the comparison of interest. Extracted when the effect size is calculated from inferential statistics.</t>
+  </si>
+  <si>
+    <t>Type of statistic (e.g., t, F). Extracted when the effect size is calculated from inferential statistics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of  tests conducted before exposure to PEI prior to the test effect of interest. </t>
+  </si>
+  <si>
+    <t>consistent = control items contain specific information from the original event; no_misinformation = control condition received no misleading PEI; neutral = control condition received information in general terms that was not inconsistent with the original</t>
+  </si>
+  <si>
+    <t>Total number of items on the test, including filler items.</t>
+  </si>
+  <si>
+    <t>Number of misled items on the test.</t>
+  </si>
+  <si>
+    <t>Number of control items on the test.</t>
+  </si>
+  <si>
+    <t>Central or peripheral details. Coded only when there is an explicit manipulation of centrality.</t>
   </si>
 </sst>
 </file>
@@ -944,17 +950,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDF0301-BBC4-4423-AE5D-86F2CEAC869C}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.73046875" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -962,13 +968,13 @@
         <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -976,10 +982,10 @@
         <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -987,10 +993,10 @@
         <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -998,10 +1004,10 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1009,10 +1015,10 @@
         <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1020,10 +1026,10 @@
         <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1031,10 +1037,10 @@
         <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1042,10 +1048,10 @@
         <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1053,10 +1059,10 @@
         <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1064,10 +1070,10 @@
         <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1075,10 +1081,10 @@
         <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1086,10 +1092,10 @@
         <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1097,10 +1103,10 @@
         <v>86</v>
       </c>
       <c r="C13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1108,10 +1114,10 @@
         <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1119,750 +1125,756 @@
         <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D20" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D23" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D24" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D25" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D26" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D30" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="C31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="C32" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>104</v>
+        <v>165</v>
       </c>
       <c r="C33" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>105</v>
+        <v>166</v>
       </c>
       <c r="C34" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>106</v>
+        <v>167</v>
       </c>
       <c r="C35" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="C36" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C37" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+      <c r="D37" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D38" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>112</v>
+        <v>170</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>113</v>
+        <v>171</v>
       </c>
       <c r="C40" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+      <c r="D41" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C43" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C45" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C47" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C48" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C49" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C50" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D50" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D51" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D52" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C53" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D53" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C54" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D54" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="C55" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C56" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D56" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>130</v>
+        <v>172</v>
       </c>
       <c r="C57" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C58" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D58" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="C60" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D60" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C61" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C62" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C63" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D63" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="C64" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C65" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C66" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D66" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C67" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D67" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C68" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D68" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C69" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D69" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="C70" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D70" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="C71" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
       <c r="C72" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>143</v>
+        <v>174</v>
       </c>
       <c r="C73" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="C74" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="C75" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="D75" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B76" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="C76" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated models, with quadratic effect of accuracy
</commit_message>
<xml_diff>
--- a/data/mema_codebook.xlsx
+++ b/data/mema_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Misinformation_meta\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RabbitSnore\Documents\Projects\Misinformation_meta\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB331700-FFAB-4D7E-A4C1-5464757E0DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B008848-8FC3-4FA7-A206-7470BACC413D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{38FE1802-D0E4-4D04-A5E5-B4F66745BCD3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{38FE1802-D0E4-4D04-A5E5-B4F66745BCD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="187">
   <si>
     <t>id_record</t>
   </si>
@@ -570,6 +570,33 @@
   </si>
   <si>
     <t>Central or peripheral details. Coded only when there is an explicit manipulation of centrality.</t>
+  </si>
+  <si>
+    <t>sd_imputed</t>
+  </si>
+  <si>
+    <t>yi</t>
+  </si>
+  <si>
+    <t>vi</t>
+  </si>
+  <si>
+    <t>control_accuracy</t>
+  </si>
+  <si>
+    <t>Accuracy in the control condition. Because this variable is calculated in the wrangling code, it is not included in the raw or cleaned data. When accuracy is reported as a proportion, this is simply the mean accuracy rate in the control condition. When accuracy is reported as a count, this value is estimated by dividing the reported mean count in the control condition by the number of critical items on the test.</t>
+  </si>
+  <si>
+    <t>Indicator for whether the SD for accuracy has been imputed.</t>
+  </si>
+  <si>
+    <t>0 = not imputed; 1 = imputed</t>
+  </si>
+  <si>
+    <t>Standardized mean difference for the misinformation effect.</t>
+  </si>
+  <si>
+    <t>Sampling variance for the standardized mean difference.</t>
   </si>
 </sst>
 </file>
@@ -948,19 +975,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDF0301-BBC4-4423-AE5D-86F2CEAC869C}">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.73046875" customWidth="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -974,7 +1001,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -985,7 +1012,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -996,7 +1023,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +1034,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1018,7 +1045,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1029,7 +1056,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1040,7 +1067,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1051,7 +1078,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1062,7 +1089,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1073,7 +1100,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1084,7 +1111,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1095,7 +1122,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1106,7 +1133,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1117,7 +1144,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1128,7 +1155,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1139,7 +1166,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1150,7 +1177,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1161,7 +1188,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1175,7 +1202,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1189,7 +1216,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1203,7 +1230,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1214,7 +1241,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1228,7 +1255,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1242,7 +1269,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1256,7 +1283,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1270,7 +1297,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1281,7 +1308,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1292,7 +1319,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1303,7 +1330,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1317,7 +1344,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1328,7 +1355,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1339,7 +1366,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1350,7 +1377,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1361,7 +1388,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1372,7 +1399,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1383,7 +1410,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1397,7 +1424,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1411,7 +1438,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1422,7 +1449,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1433,7 +1460,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1447,7 +1474,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1458,7 +1485,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1469,7 +1496,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1480,7 +1507,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1491,7 +1518,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1502,7 +1529,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1513,7 +1540,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1524,7 +1551,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1535,7 +1562,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1549,7 +1576,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1563,7 +1590,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1577,7 +1604,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1591,7 +1618,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1605,7 +1632,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1616,7 +1643,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1630,7 +1657,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1641,7 +1668,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1655,7 +1682,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1666,7 +1693,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1680,7 +1707,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1691,7 +1718,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1702,7 +1729,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1716,7 +1743,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1727,7 +1754,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -1738,7 +1765,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1752,7 +1779,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1766,7 +1793,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -1780,7 +1807,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -1794,7 +1821,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -1808,7 +1835,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1819,7 +1846,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -1830,7 +1857,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -1841,7 +1868,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -1852,7 +1879,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>154</v>
       </c>
@@ -1866,7 +1893,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>155</v>
       </c>
@@ -1875,6 +1902,53 @@
       </c>
       <c r="C76" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>178</v>
+      </c>
+      <c r="B77" t="s">
+        <v>183</v>
+      </c>
+      <c r="C77" t="s">
+        <v>132</v>
+      </c>
+      <c r="D77" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>179</v>
+      </c>
+      <c r="B78" t="s">
+        <v>185</v>
+      </c>
+      <c r="C78" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>180</v>
+      </c>
+      <c r="B79" t="s">
+        <v>186</v>
+      </c>
+      <c r="C79" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>181</v>
+      </c>
+      <c r="B80" t="s">
+        <v>182</v>
+      </c>
+      <c r="C80" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>